<commit_message>
experiment results on excel filled
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspaces\python\copt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47995F3E-B5B8-42C7-85B8-2083D1490DB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B9F1CD-3F9B-4CEB-A31D-D03CB261B57B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14655" activeTab="2" xr2:uid="{52A98BD8-4E11-A341-8E33-FFC30D64FA33}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14655" xr2:uid="{52A98BD8-4E11-A341-8E33-FFC30D64FA33}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -315,18 +315,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -334,6 +329,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1840,7 +1840,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2097890644945304E-2</c:v>
+                  <c:v>2.1435556047957841E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1967,22 +1967,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.694295230943992</c:v>
+                  <c:v>0.28803018926047863</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4201044336114379E-2</c:v>
+                  <c:v>3.3177421530279964E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.7500926709926138E-2</c:v>
+                  <c:v>1.6827101290370412E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9112597344432506E-2</c:v>
+                  <c:v>8.688465751412652E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.9162718628144977E-3</c:v>
+                  <c:v>5.6246789245780558E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2603,37 +2603,37 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.7109000000000001</c:v>
+                  <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1773999999999996</c:v>
+                  <c:v>3.5937999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0217999999999998</c:v>
+                  <c:v>5.7656000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.732300000000002</c:v>
+                  <c:v>35.382899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75.835999999999999</c:v>
+                  <c:v>64.046899999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>216.99979999999999</c:v>
+                  <c:v>188.39060000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>239.67930000000001</c:v>
+                  <c:v>216.10939999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>355.51</c:v>
+                  <c:v>311.26560000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>408.69720000000001</c:v>
+                  <c:v>365.04689999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1723.3974000000001</c:v>
+                  <c:v>1575.6561999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4375.9088000000002</c:v>
+                  <c:v>2794.1891000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2736,37 +2736,37 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.1263000000000001</c:v>
+                  <c:v>1.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3170999999999999</c:v>
+                  <c:v>4.4062000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0927000000000007</c:v>
+                  <c:v>7.5156000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.798900000000003</c:v>
+                  <c:v>44.488599999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.647000000000006</c:v>
+                  <c:v>80.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>264.70929999999998</c:v>
+                  <c:v>224.54689999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>306.41160000000002</c:v>
+                  <c:v>271.32810000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>440.51830000000001</c:v>
+                  <c:v>387.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>524.71289999999999</c:v>
+                  <c:v>440.04689999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2735.4942999999998</c:v>
+                  <c:v>2883.3281000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6280.2394000000004</c:v>
+                  <c:v>3410.9778999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2899,7 +2899,7 @@
                   <c:v>1655.0168000000001</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="#,##0.00">
-                  <c:v>2945.4787999999999</c:v>
+                  <c:v>3689.8222000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3032,7 +3032,7 @@
                   <c:v>2248.9456</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="#,##0.00">
-                  <c:v>4131.8188</c:v>
+                  <c:v>5671.4978000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5562,13 +5562,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>38106</xdr:colOff>
+      <xdr:colOff>66681</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>117475</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -5897,8 +5897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EEADE2-A9B3-674B-BA9B-72229A521D77}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6339,7 +6339,7 @@
   <dimension ref="A2:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G10"/>
+      <selection activeCell="L9" sqref="L9:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6392,7 +6392,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -6442,7 +6442,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -6490,7 +6490,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -6540,7 +6540,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -6588,7 +6588,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -6638,7 +6638,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -6686,179 +6686,182 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="15">
         <f t="shared" ref="C9:P9" si="0">100*((C4-C6)/C4)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="15">
         <f t="shared" si="0"/>
         <v>0.28331679676410071</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="15">
         <f t="shared" si="0"/>
         <v>6.6721378395387205</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="15">
         <f t="shared" si="0"/>
         <v>1.4825105598988066E-2</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="15">
         <f t="shared" si="0"/>
         <v>0.21084435931048381</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="15">
         <f t="shared" si="0"/>
         <v>0.12111948505301814</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="15">
         <f t="shared" si="0"/>
         <v>4.0020902606961082</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="15">
         <f t="shared" si="0"/>
         <v>8.8497113987194301E-2</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="15">
         <f t="shared" si="0"/>
         <v>16.735867692541735</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="15">
         <f t="shared" si="0"/>
         <v>2.5065027300464802E-2</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="15">
         <f t="shared" si="0"/>
         <v>2.4661736476073174E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="15">
         <f t="shared" ref="C11:P11" si="1">100*((C4-C8)/C4)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="15">
         <f t="shared" si="1"/>
         <v>1.0851631997006446</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="15">
         <f t="shared" si="1"/>
         <v>2.3672346037093849E-2</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="15">
         <f t="shared" si="1"/>
         <v>2.3495459874602515E-2</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="15">
         <f t="shared" si="1"/>
         <v>4.1650458033726358E-3</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="15">
         <f t="shared" si="1"/>
         <v>7.0374062210216401E-2</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="15">
         <f t="shared" si="1"/>
         <v>1.1870917907007463E-3</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="15">
         <f t="shared" si="1"/>
         <v>1.0179336691022478E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E11:E12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
@@ -6875,17 +6878,14 @@
     <mergeCell ref="P11:P12"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="N11:N12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6897,11 +6897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F31A019-EF8C-8649-B7F3-D195899C8CF2}">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6912,50 +6912,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18" t="s">
+      <c r="L1" s="20"/>
+      <c r="M1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18" t="s">
+      <c r="N1" s="20"/>
+      <c r="O1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18" t="s">
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18" t="s">
+      <c r="R1" s="20"/>
+      <c r="S1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18" t="s">
+      <c r="T1" s="20"/>
+      <c r="U1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18" t="s">
+      <c r="V1" s="20"/>
+      <c r="W1" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="18"/>
+      <c r="X1" s="20"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C2" s="10" t="s">
@@ -7026,7 +7026,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -7035,52 +7035,52 @@
       <c r="C3" s="13">
         <v>1.5461</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>1.9312</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>3.9401000000000002</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <v>5.1288999999999998</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>6.3446999999999996</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>8.5748999999999995</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>38.189</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <v>48.531300000000002</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="12">
         <v>72.674499999999995</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="12">
         <v>93.75</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="12">
         <v>161.48249999999999</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="12">
         <v>225.67140000000001</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="12">
         <v>223.24950000000001</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="12">
         <v>301.35610000000003</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="12">
         <v>324.71039999999999</v>
       </c>
-      <c r="R3" s="13">
+      <c r="R3" s="12">
         <v>478.46609999999998</v>
       </c>
-      <c r="S3" s="13">
+      <c r="S3" s="12">
         <v>464.81439999999998</v>
       </c>
       <c r="T3" s="13">
@@ -7093,1283 +7093,1354 @@
         <v>2248.9456</v>
       </c>
       <c r="W3" s="13">
-        <v>2945.4787999999999</v>
+        <v>3689.8222000000001</v>
       </c>
       <c r="X3" s="13">
-        <v>4131.8188</v>
+        <v>5671.4978000000001</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>15141</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>15141</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>18464</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>18464</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>63096</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <v>63096</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <v>87747</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <v>87747</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>329480</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <v>329480</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <v>779085</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="11">
         <v>779085</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="11">
         <v>1673454</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="11">
         <v>1673454</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <v>1660792</v>
       </c>
-      <c r="R4" s="12">
+      <c r="R4" s="11">
         <v>1660768</v>
       </c>
-      <c r="S4" s="12">
+      <c r="S4" s="11">
         <v>2050264</v>
       </c>
-      <c r="T4" s="12">
+      <c r="T4" s="11">
         <v>2050264</v>
       </c>
-      <c r="U4" s="12">
+      <c r="U4" s="11">
         <v>5800740</v>
       </c>
-      <c r="V4" s="12">
+      <c r="V4" s="11">
         <v>5800794</v>
       </c>
-      <c r="W4" s="12">
+      <c r="W4" s="11">
         <v>4800274</v>
       </c>
-      <c r="X4" s="12">
+      <c r="X4" s="11">
         <v>4800274</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>0.67100000000000004</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.39979999999999999</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>1.6584000000000001</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>1.1163000000000001</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>2.7709999999999999</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>1.3845000000000001</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>15.633800000000001</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>8.7070000000000007</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>32.877600000000001</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>14.837</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <v>64.142099999999999</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="12">
         <v>35.283999999999999</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <v>70.239199999999997</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="12">
         <v>33.219700000000003</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="12">
         <v>128.3947</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="12">
         <v>63.618000000000002</v>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="12">
         <v>142.79310000000001</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="12">
         <v>61.295900000000003</v>
       </c>
-      <c r="U5" s="13">
+      <c r="U5" s="12">
         <v>903.16920000000005</v>
       </c>
-      <c r="V5" s="13">
+      <c r="V5" s="12">
         <v>448.58699999999999</v>
       </c>
-      <c r="W5" s="13">
+      <c r="W5" s="12">
         <v>2534.8456999999999</v>
       </c>
-      <c r="X5" s="13">
+      <c r="X5" s="12">
         <v>1474.5264</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>15141</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>15141</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>18464</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>18464</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>62916</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <v>62916</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>87747</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="11">
         <v>87747</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="11">
         <v>329468</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="11">
         <v>329468</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="11">
         <v>732261</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="11">
         <v>732261</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="11">
         <v>1667254</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P6" s="11">
         <v>1667254</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="Q6" s="11">
         <v>1655326</v>
       </c>
-      <c r="R6" s="12">
+      <c r="R6" s="11">
         <v>1655326</v>
       </c>
-      <c r="S6" s="12">
+      <c r="S6" s="11">
         <v>2029337</v>
       </c>
-      <c r="T6" s="12">
+      <c r="T6" s="11">
         <v>2029337</v>
       </c>
-      <c r="U6" s="12">
+      <c r="U6" s="11">
         <v>5775888</v>
       </c>
-      <c r="V6" s="12">
+      <c r="V6" s="11">
         <v>5775888</v>
       </c>
-      <c r="W6" s="12">
+      <c r="W6" s="11">
         <v>4800274</v>
       </c>
-      <c r="X6" s="12">
+      <c r="X6" s="11">
         <v>4800274</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="11">
-        <v>1.7109000000000001</v>
-      </c>
-      <c r="D7" s="11">
-        <v>2.1263000000000001</v>
-      </c>
-      <c r="E7" s="11">
-        <v>4.1773999999999996</v>
-      </c>
-      <c r="F7" s="11">
-        <v>5.3170999999999999</v>
-      </c>
-      <c r="G7" s="11">
-        <v>7.0217999999999998</v>
-      </c>
-      <c r="H7" s="11">
-        <v>9.0927000000000007</v>
-      </c>
-      <c r="I7" s="11">
-        <v>40.732300000000002</v>
-      </c>
-      <c r="J7" s="11">
-        <v>52.798900000000003</v>
-      </c>
-      <c r="K7" s="11">
-        <v>75.835999999999999</v>
-      </c>
-      <c r="L7" s="11">
-        <v>97.647000000000006</v>
-      </c>
-      <c r="M7" s="11">
-        <v>216.99979999999999</v>
-      </c>
-      <c r="N7" s="11">
-        <v>264.70929999999998</v>
-      </c>
-      <c r="O7" s="11">
-        <v>239.67930000000001</v>
-      </c>
-      <c r="P7" s="11">
-        <v>306.41160000000002</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>355.51</v>
-      </c>
-      <c r="R7" s="11">
-        <v>440.51830000000001</v>
-      </c>
-      <c r="S7" s="11">
-        <v>408.69720000000001</v>
-      </c>
-      <c r="T7" s="11">
-        <v>524.71289999999999</v>
-      </c>
-      <c r="U7" s="11">
-        <v>1723.3974000000001</v>
-      </c>
-      <c r="V7" s="11">
-        <v>2735.4942999999998</v>
-      </c>
-      <c r="W7" s="11">
-        <v>4375.9088000000002</v>
-      </c>
-      <c r="X7" s="11">
-        <v>6280.2394000000004</v>
+      <c r="C7" s="13">
+        <v>1.625</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1.875</v>
+      </c>
+      <c r="E7" s="13">
+        <v>3.5937999999999999</v>
+      </c>
+      <c r="F7" s="13">
+        <v>4.4062000000000001</v>
+      </c>
+      <c r="G7" s="13">
+        <v>5.7656000000000001</v>
+      </c>
+      <c r="H7" s="13">
+        <v>7.5156000000000001</v>
+      </c>
+      <c r="I7" s="13">
+        <v>35.382899999999999</v>
+      </c>
+      <c r="J7" s="13">
+        <v>44.488599999999998</v>
+      </c>
+      <c r="K7" s="13">
+        <v>64.046899999999994</v>
+      </c>
+      <c r="L7" s="13">
+        <v>80.75</v>
+      </c>
+      <c r="M7" s="13">
+        <v>188.39060000000001</v>
+      </c>
+      <c r="N7" s="13">
+        <v>224.54689999999999</v>
+      </c>
+      <c r="O7" s="13">
+        <v>216.10939999999999</v>
+      </c>
+      <c r="P7" s="13">
+        <v>271.32810000000001</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>311.26560000000001</v>
+      </c>
+      <c r="R7" s="13">
+        <v>387.5</v>
+      </c>
+      <c r="S7" s="13">
+        <v>365.04689999999999</v>
+      </c>
+      <c r="T7" s="13">
+        <v>440.04689999999999</v>
+      </c>
+      <c r="U7" s="13">
+        <v>1575.6561999999999</v>
+      </c>
+      <c r="V7" s="13">
+        <v>2883.3281000000002</v>
+      </c>
+      <c r="W7" s="13">
+        <v>2794.1891000000001</v>
+      </c>
+      <c r="X7" s="13">
+        <v>3410.9778999999999</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>15141</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>15141</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>18464</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>18464</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>63096</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>63096</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>87747</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="11">
         <v>87747</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="11">
         <v>329480</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <v>329480</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="11">
         <v>776907</v>
       </c>
-      <c r="N8" s="12">
-        <v>765885</v>
-      </c>
-      <c r="O8" s="12">
+      <c r="N8" s="11">
+        <v>776841</v>
+      </c>
+      <c r="O8" s="11">
         <v>1673454</v>
       </c>
-      <c r="P8" s="12">
+      <c r="P8" s="11">
         <v>1673454</v>
       </c>
-      <c r="Q8" s="12">
-        <v>1660425</v>
-      </c>
-      <c r="R8" s="12">
-        <v>1660200</v>
-      </c>
-      <c r="S8" s="12">
+      <c r="Q8" s="11">
+        <v>1660436</v>
+      </c>
+      <c r="R8" s="11">
+        <v>1660217</v>
+      </c>
+      <c r="S8" s="11">
         <v>2050264</v>
       </c>
-      <c r="T8" s="12">
-        <v>2048470</v>
-      </c>
-      <c r="U8" s="12">
+      <c r="T8" s="11">
+        <v>2049919</v>
+      </c>
+      <c r="U8" s="11">
         <v>5800794</v>
       </c>
-      <c r="V8" s="12">
-        <v>5797365</v>
-      </c>
-      <c r="W8" s="12">
+      <c r="V8" s="11">
+        <v>5800290</v>
+      </c>
+      <c r="W8" s="11">
         <v>4800274</v>
       </c>
-      <c r="X8" s="12">
-        <v>4799942</v>
+      <c r="X8" s="11">
+        <v>4800004</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="19">
         <f>100*(C4-C6)/C4</f>
         <v>0</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="19">
         <f t="shared" ref="D9:X9" si="0">100*(D4-D6)/D4</f>
         <v>0</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="19">
         <f t="shared" si="0"/>
         <v>0.28527957398250287</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="19">
         <f t="shared" si="0"/>
         <v>0.28527957398250287</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="19">
         <f t="shared" si="0"/>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="19">
         <f t="shared" si="0"/>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="19">
         <f t="shared" si="0"/>
         <v>6.0101272646758694</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="19">
         <f t="shared" si="0"/>
         <v>6.0101272646758694</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O9" s="19">
         <f t="shared" si="0"/>
         <v>0.37049121158992121</v>
       </c>
-      <c r="P9" s="17">
+      <c r="P9" s="19">
         <f t="shared" si="0"/>
         <v>0.37049121158992121</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="Q9" s="19">
         <f t="shared" si="0"/>
         <v>0.32912008246667857</v>
       </c>
-      <c r="R9" s="17">
+      <c r="R9" s="19">
         <f t="shared" si="0"/>
         <v>0.32767972407946205</v>
       </c>
-      <c r="S9" s="17">
+      <c r="S9" s="19">
         <f t="shared" si="0"/>
         <v>1.020697822329222</v>
       </c>
-      <c r="T9" s="17">
+      <c r="T9" s="19">
         <f t="shared" si="0"/>
         <v>1.020697822329222</v>
       </c>
-      <c r="U9" s="17">
+      <c r="U9" s="19">
         <f t="shared" si="0"/>
         <v>0.42842809710485213</v>
       </c>
-      <c r="V9" s="17">
+      <c r="V9" s="19">
         <f t="shared" si="0"/>
         <v>0.42935501588230851</v>
       </c>
-      <c r="W9" s="17">
+      <c r="W9" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X9" s="17">
+      <c r="X9" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="18">
         <f>100*(C4-C8)/C4</f>
         <v>0</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="18">
         <f t="shared" ref="D11:X11" si="1">100*(D4-D8)/D4</f>
         <v>0</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="18">
         <f t="shared" si="1"/>
         <v>0.27955871310575869</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="18">
         <f t="shared" si="1"/>
-        <v>1.694295230943992</v>
-      </c>
-      <c r="O11" s="16">
+        <v>0.28803018926047863</v>
+      </c>
+      <c r="O11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="Q11" s="18">
         <f t="shared" si="1"/>
-        <v>2.2097890644945304E-2</v>
-      </c>
-      <c r="R11" s="16">
+        <v>2.1435556047957841E-2</v>
+      </c>
+      <c r="R11" s="18">
         <f t="shared" si="1"/>
-        <v>3.4201044336114379E-2</v>
-      </c>
-      <c r="S11" s="16">
+        <v>3.3177421530279964E-2</v>
+      </c>
+      <c r="S11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T11" s="16">
+      <c r="T11" s="18">
         <f t="shared" si="1"/>
-        <v>8.7500926709926138E-2</v>
-      </c>
-      <c r="U11" s="16">
+        <v>1.6827101290370412E-2</v>
+      </c>
+      <c r="U11" s="18">
         <f t="shared" si="1"/>
         <v>-9.3091571075414514E-4</v>
       </c>
-      <c r="V11" s="16">
+      <c r="V11" s="18">
         <f t="shared" si="1"/>
-        <v>5.9112597344432506E-2</v>
-      </c>
-      <c r="W11" s="16">
+        <v>8.688465751412652E-3</v>
+      </c>
+      <c r="W11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X11" s="16">
+      <c r="X11" s="18">
         <f t="shared" si="1"/>
-        <v>6.9162718628144977E-3</v>
+        <v>5.6246789245780558E-3</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="16">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16">
         <f>E9</f>
         <v>0</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19">
+      <c r="F14" s="16"/>
+      <c r="G14" s="16">
         <f>G9</f>
         <v>0.28527957398250287</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16">
         <f>I9</f>
         <v>0</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19">
+      <c r="J14" s="16"/>
+      <c r="K14" s="16">
         <f>K9</f>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19">
+      <c r="L14" s="16"/>
+      <c r="M14" s="16">
         <f>M9</f>
         <v>6.0101272646758694</v>
       </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="19">
+      <c r="N14" s="17"/>
+      <c r="O14" s="16">
         <f>O9</f>
         <v>0.37049121158992121</v>
       </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="19">
+      <c r="P14" s="17"/>
+      <c r="Q14" s="16">
         <f>Q9</f>
         <v>0.32912008246667857</v>
       </c>
-      <c r="R14" s="20"/>
-      <c r="S14" s="19">
+      <c r="R14" s="17"/>
+      <c r="S14" s="16">
         <f>S9</f>
         <v>1.020697822329222</v>
       </c>
-      <c r="T14" s="20"/>
-      <c r="U14" s="19">
+      <c r="T14" s="17"/>
+      <c r="U14" s="16">
         <f>U9</f>
         <v>0.42842809710485213</v>
       </c>
-      <c r="V14" s="20"/>
-      <c r="W14" s="19">
+      <c r="V14" s="17"/>
+      <c r="W14" s="16">
         <f>W9</f>
         <v>0</v>
       </c>
-      <c r="X14" s="20"/>
+      <c r="X14" s="17"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="14"/>
       <c r="B15" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="16">
         <f>D9</f>
         <v>0</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16">
         <f>F9</f>
         <v>0</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19">
+      <c r="F15" s="16"/>
+      <c r="G15" s="16">
         <f>H9</f>
         <v>0.28527957398250287</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19">
+      <c r="H15" s="16"/>
+      <c r="I15" s="16">
         <f>J9</f>
         <v>0</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19">
+      <c r="J15" s="16"/>
+      <c r="K15" s="16">
         <f>L9</f>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19">
+      <c r="L15" s="16"/>
+      <c r="M15" s="16">
         <f>N9</f>
         <v>6.0101272646758694</v>
       </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="19">
+      <c r="N15" s="17"/>
+      <c r="O15" s="16">
         <f>P9</f>
         <v>0.37049121158992121</v>
       </c>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="19">
+      <c r="P15" s="17"/>
+      <c r="Q15" s="16">
         <f>R9</f>
         <v>0.32767972407946205</v>
       </c>
-      <c r="R15" s="20"/>
-      <c r="S15" s="19">
+      <c r="R15" s="17"/>
+      <c r="S15" s="16">
         <f>T9</f>
         <v>1.020697822329222</v>
       </c>
-      <c r="T15" s="20"/>
-      <c r="U15" s="19">
+      <c r="T15" s="17"/>
+      <c r="U15" s="16">
         <f>V9</f>
         <v>0.42935501588230851</v>
       </c>
-      <c r="V15" s="20"/>
-      <c r="W15" s="19">
+      <c r="V15" s="17"/>
+      <c r="W15" s="16">
         <f>X9</f>
         <v>0</v>
       </c>
-      <c r="X15" s="20"/>
+      <c r="X15" s="17"/>
     </row>
     <row r="17" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="16">
         <f>C11</f>
         <v>0</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19">
+      <c r="D17" s="16"/>
+      <c r="E17" s="16">
         <f>E11</f>
         <v>0</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16">
         <f>G11</f>
         <v>0</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19">
+      <c r="H17" s="16"/>
+      <c r="I17" s="16">
         <f>I11</f>
         <v>0</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19">
+      <c r="J17" s="16"/>
+      <c r="K17" s="16">
         <f>K11</f>
         <v>0</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19">
+      <c r="L17" s="16"/>
+      <c r="M17" s="16">
         <f>M11</f>
         <v>0.27955871310575869</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19">
+      <c r="N17" s="16"/>
+      <c r="O17" s="16">
         <f>O11</f>
         <v>0</v>
       </c>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19">
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16">
         <f>Q11</f>
-        <v>2.2097890644945304E-2</v>
-      </c>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19">
+        <v>2.1435556047957841E-2</v>
+      </c>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16">
         <f>S11</f>
         <v>0</v>
       </c>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19">
+      <c r="T17" s="16"/>
+      <c r="U17" s="16">
         <f>U11</f>
         <v>-9.3091571075414514E-4</v>
       </c>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19">
+      <c r="V17" s="16"/>
+      <c r="W17" s="16">
         <f>W11</f>
         <v>0</v>
       </c>
-      <c r="X17" s="19"/>
+      <c r="X17" s="16"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="16">
         <f>D12</f>
         <v>0</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19">
+      <c r="D18" s="16"/>
+      <c r="E18" s="16">
         <f>F12</f>
         <v>0</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19">
+      <c r="F18" s="16"/>
+      <c r="G18" s="16">
         <f>H11</f>
         <v>0</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19">
+      <c r="H18" s="16"/>
+      <c r="I18" s="16">
         <f>J11</f>
         <v>0</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19">
+      <c r="J18" s="16"/>
+      <c r="K18" s="16">
         <f>L11</f>
         <v>0</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19">
+      <c r="L18" s="16"/>
+      <c r="M18" s="16">
         <f>N11</f>
-        <v>1.694295230943992</v>
-      </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19">
+        <v>0.28803018926047863</v>
+      </c>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16">
         <f>P11</f>
         <v>0</v>
       </c>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19">
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16">
         <f>R11</f>
-        <v>3.4201044336114379E-2</v>
-      </c>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19">
+        <v>3.3177421530279964E-2</v>
+      </c>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16">
         <f>T11</f>
-        <v>8.7500926709926138E-2</v>
-      </c>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19">
+        <v>1.6827101290370412E-2</v>
+      </c>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16">
         <f>V11</f>
-        <v>5.9112597344432506E-2</v>
-      </c>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19">
+        <v>8.688465751412652E-3</v>
+      </c>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16">
         <f>X11</f>
-        <v>6.9162718628144977E-3</v>
-      </c>
-      <c r="X18" s="19"/>
+        <v>5.6246789245780558E-3</v>
+      </c>
+      <c r="X18" s="16"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="16">
         <f>C5</f>
         <v>0.67100000000000004</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19">
+      <c r="D20" s="16"/>
+      <c r="E20" s="16">
         <f>E5</f>
         <v>1.6584000000000001</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19">
+      <c r="F20" s="16"/>
+      <c r="G20" s="16">
         <f>G5</f>
         <v>2.7709999999999999</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19">
+      <c r="H20" s="16"/>
+      <c r="I20" s="16">
         <f>I5</f>
         <v>15.633800000000001</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19">
+      <c r="J20" s="16"/>
+      <c r="K20" s="16">
         <f>K5</f>
         <v>32.877600000000001</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19">
+      <c r="L20" s="16"/>
+      <c r="M20" s="16">
         <f>M5</f>
         <v>64.142099999999999</v>
       </c>
-      <c r="N20" s="20"/>
-      <c r="O20" s="19">
+      <c r="N20" s="17"/>
+      <c r="O20" s="16">
         <f>O5</f>
         <v>70.239199999999997</v>
       </c>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="19">
+      <c r="P20" s="17"/>
+      <c r="Q20" s="16">
         <f>Q5</f>
         <v>128.3947</v>
       </c>
-      <c r="R20" s="20"/>
-      <c r="S20" s="19">
+      <c r="R20" s="17"/>
+      <c r="S20" s="16">
         <f>S5</f>
         <v>142.79310000000001</v>
       </c>
-      <c r="T20" s="20"/>
-      <c r="U20" s="19">
+      <c r="T20" s="17"/>
+      <c r="U20" s="16">
         <f>U5</f>
         <v>903.16920000000005</v>
       </c>
-      <c r="V20" s="20"/>
-      <c r="W20" s="19">
+      <c r="V20" s="17"/>
+      <c r="W20" s="16">
         <f>W5</f>
         <v>2534.8456999999999</v>
       </c>
-      <c r="X20" s="20"/>
+      <c r="X20" s="17"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="14"/>
       <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="16">
         <f>D5</f>
         <v>0.39979999999999999</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19">
+      <c r="D21" s="16"/>
+      <c r="E21" s="16">
         <f>F5</f>
         <v>1.1163000000000001</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16">
         <f>H5</f>
         <v>1.3845000000000001</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19">
+      <c r="H21" s="16"/>
+      <c r="I21" s="16">
         <f>J5</f>
         <v>8.7070000000000007</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19">
+      <c r="J21" s="16"/>
+      <c r="K21" s="16">
         <f>L5</f>
         <v>14.837</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19">
+      <c r="L21" s="16"/>
+      <c r="M21" s="16">
         <f>N5</f>
         <v>35.283999999999999</v>
       </c>
-      <c r="N21" s="20"/>
-      <c r="O21" s="19">
+      <c r="N21" s="17"/>
+      <c r="O21" s="16">
         <f>P5</f>
         <v>33.219700000000003</v>
       </c>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="19">
+      <c r="P21" s="17"/>
+      <c r="Q21" s="16">
         <f>R5</f>
         <v>63.618000000000002</v>
       </c>
-      <c r="R21" s="20"/>
-      <c r="S21" s="19">
+      <c r="R21" s="17"/>
+      <c r="S21" s="16">
         <f>T5</f>
         <v>61.295900000000003</v>
       </c>
-      <c r="T21" s="20"/>
-      <c r="U21" s="19">
+      <c r="T21" s="17"/>
+      <c r="U21" s="16">
         <f>V5</f>
         <v>448.58699999999999</v>
       </c>
-      <c r="V21" s="20"/>
-      <c r="W21" s="19">
+      <c r="V21" s="17"/>
+      <c r="W21" s="16">
         <f>X5</f>
         <v>1474.5264</v>
       </c>
-      <c r="X21" s="20"/>
+      <c r="X21" s="17"/>
     </row>
     <row r="23" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="16">
         <f>C7</f>
-        <v>1.7109000000000001</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19">
+        <v>1.625</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16">
         <f>E7</f>
-        <v>4.1773999999999996</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19">
+        <v>3.5937999999999999</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16">
         <f>G7</f>
-        <v>7.0217999999999998</v>
-      </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19">
+        <v>5.7656000000000001</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16">
         <f>I7</f>
-        <v>40.732300000000002</v>
-      </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19">
+        <v>35.382899999999999</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16">
         <f>K7</f>
-        <v>75.835999999999999</v>
-      </c>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19">
+        <v>64.046899999999994</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16">
         <f>M7</f>
-        <v>216.99979999999999</v>
-      </c>
-      <c r="N23" s="20"/>
-      <c r="O23" s="19">
+        <v>188.39060000000001</v>
+      </c>
+      <c r="N23" s="17"/>
+      <c r="O23" s="16">
         <f>O7</f>
-        <v>239.67930000000001</v>
-      </c>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="19">
+        <v>216.10939999999999</v>
+      </c>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="16">
         <f>Q7</f>
-        <v>355.51</v>
-      </c>
-      <c r="R23" s="20"/>
-      <c r="S23" s="19">
+        <v>311.26560000000001</v>
+      </c>
+      <c r="R23" s="17"/>
+      <c r="S23" s="16">
         <f>S7</f>
-        <v>408.69720000000001</v>
-      </c>
-      <c r="T23" s="20"/>
-      <c r="U23" s="19">
+        <v>365.04689999999999</v>
+      </c>
+      <c r="T23" s="17"/>
+      <c r="U23" s="16">
         <f>U7</f>
-        <v>1723.3974000000001</v>
-      </c>
-      <c r="V23" s="20"/>
-      <c r="W23" s="19">
+        <v>1575.6561999999999</v>
+      </c>
+      <c r="V23" s="17"/>
+      <c r="W23" s="16">
         <f>W7</f>
-        <v>4375.9088000000002</v>
-      </c>
-      <c r="X23" s="20"/>
+        <v>2794.1891000000001</v>
+      </c>
+      <c r="X23" s="17"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="14"/>
       <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="16">
         <f>D7</f>
-        <v>2.1263000000000001</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19">
+        <v>1.875</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16">
         <f>F7</f>
-        <v>5.3170999999999999</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19">
+        <v>4.4062000000000001</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16">
         <f>H7</f>
-        <v>9.0927000000000007</v>
-      </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19">
+        <v>7.5156000000000001</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16">
         <f>J7</f>
-        <v>52.798900000000003</v>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19">
+        <v>44.488599999999998</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16">
         <f>L7</f>
-        <v>97.647000000000006</v>
-      </c>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19">
+        <v>80.75</v>
+      </c>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16">
         <f>N7</f>
-        <v>264.70929999999998</v>
-      </c>
-      <c r="N24" s="20"/>
-      <c r="O24" s="19">
+        <v>224.54689999999999</v>
+      </c>
+      <c r="N24" s="17"/>
+      <c r="O24" s="16">
         <f>P7</f>
-        <v>306.41160000000002</v>
-      </c>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="19">
+        <v>271.32810000000001</v>
+      </c>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="16">
         <f>R7</f>
-        <v>440.51830000000001</v>
-      </c>
-      <c r="R24" s="20"/>
-      <c r="S24" s="19">
+        <v>387.5</v>
+      </c>
+      <c r="R24" s="17"/>
+      <c r="S24" s="16">
         <f>T7</f>
-        <v>524.71289999999999</v>
-      </c>
-      <c r="T24" s="20"/>
-      <c r="U24" s="19">
+        <v>440.04689999999999</v>
+      </c>
+      <c r="T24" s="17"/>
+      <c r="U24" s="16">
         <f>V7</f>
-        <v>2735.4942999999998</v>
-      </c>
-      <c r="V24" s="20"/>
-      <c r="W24" s="19">
+        <v>2883.3281000000002</v>
+      </c>
+      <c r="V24" s="17"/>
+      <c r="W24" s="16">
         <f>X7</f>
-        <v>6280.2394000000004</v>
-      </c>
-      <c r="X24" s="20"/>
+        <v>3410.9778999999999</v>
+      </c>
+      <c r="X24" s="17"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="16">
         <f>C3</f>
         <v>1.5461</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="19">
+      <c r="D26" s="17"/>
+      <c r="E26" s="16">
         <f>E3</f>
         <v>3.9401000000000002</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="19">
+      <c r="F26" s="17"/>
+      <c r="G26" s="16">
         <f>G3</f>
         <v>6.3446999999999996</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="19">
+      <c r="H26" s="17"/>
+      <c r="I26" s="16">
         <f>I3</f>
         <v>38.189</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="19">
+      <c r="J26" s="17"/>
+      <c r="K26" s="16">
         <f>K3</f>
         <v>72.674499999999995</v>
       </c>
-      <c r="L26" s="20"/>
-      <c r="M26" s="19">
+      <c r="L26" s="17"/>
+      <c r="M26" s="16">
         <f>M3</f>
         <v>161.48249999999999</v>
       </c>
-      <c r="N26" s="20"/>
-      <c r="O26" s="19">
+      <c r="N26" s="17"/>
+      <c r="O26" s="16">
         <f>O3</f>
         <v>223.24950000000001</v>
       </c>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="19">
+      <c r="P26" s="17"/>
+      <c r="Q26" s="16">
         <f>Q3</f>
         <v>324.71039999999999</v>
       </c>
-      <c r="R26" s="20"/>
-      <c r="S26" s="19">
+      <c r="R26" s="17"/>
+      <c r="S26" s="16">
         <f>S3</f>
         <v>464.81439999999998</v>
       </c>
-      <c r="T26" s="20"/>
-      <c r="U26" s="19">
+      <c r="T26" s="17"/>
+      <c r="U26" s="16">
         <f>U3</f>
         <v>1655.0168000000001</v>
       </c>
-      <c r="V26" s="20"/>
-      <c r="W26" s="19">
+      <c r="V26" s="17"/>
+      <c r="W26" s="16">
         <f>W3</f>
-        <v>2945.4787999999999</v>
-      </c>
-      <c r="X26" s="20"/>
+        <v>3689.8222000000001</v>
+      </c>
+      <c r="X26" s="17"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="A27" s="14"/>
       <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="16">
         <f>D3</f>
         <v>1.9312</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="19">
+      <c r="D27" s="17"/>
+      <c r="E27" s="16">
         <f>F3</f>
         <v>5.1288999999999998</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="19">
+      <c r="F27" s="17"/>
+      <c r="G27" s="16">
         <f>H3</f>
         <v>8.5748999999999995</v>
       </c>
-      <c r="H27" s="20"/>
-      <c r="I27" s="19">
+      <c r="H27" s="17"/>
+      <c r="I27" s="16">
         <f>J3</f>
         <v>48.531300000000002</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="19">
+      <c r="J27" s="17"/>
+      <c r="K27" s="16">
         <f>L3</f>
         <v>93.75</v>
       </c>
-      <c r="L27" s="20"/>
-      <c r="M27" s="19">
+      <c r="L27" s="17"/>
+      <c r="M27" s="16">
         <f>N3</f>
         <v>225.67140000000001</v>
       </c>
-      <c r="N27" s="20"/>
-      <c r="O27" s="19">
+      <c r="N27" s="17"/>
+      <c r="O27" s="16">
         <f>P3</f>
         <v>301.35610000000003</v>
       </c>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="19">
+      <c r="P27" s="17"/>
+      <c r="Q27" s="16">
         <f>R3</f>
         <v>478.46609999999998</v>
       </c>
-      <c r="R27" s="20"/>
-      <c r="S27" s="19">
+      <c r="R27" s="17"/>
+      <c r="S27" s="16">
         <f>T3</f>
         <v>580.44349999999997</v>
       </c>
-      <c r="T27" s="20"/>
-      <c r="U27" s="19">
+      <c r="T27" s="17"/>
+      <c r="U27" s="16">
         <f>V3</f>
         <v>2248.9456</v>
       </c>
-      <c r="V27" s="20"/>
-      <c r="W27" s="19">
+      <c r="V27" s="17"/>
+      <c r="W27" s="16">
         <f>X3</f>
-        <v>4131.8188</v>
-      </c>
-      <c r="X27" s="20"/>
+        <v>5671.4978000000001</v>
+      </c>
+      <c r="X27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="177">
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
@@ -8394,118 +8465,47 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="I27:J27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sorting optimization on greedy
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspaces\python\copt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B9F1CD-3F9B-4CEB-A31D-D03CB261B57B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEC114C-F1E0-4405-A9DA-0934906677BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14655" xr2:uid="{52A98BD8-4E11-A341-8E33-FFC30D64FA33}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14655" activeTab="1" xr2:uid="{52A98BD8-4E11-A341-8E33-FFC30D64FA33}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -319,9 +319,14 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -329,11 +334,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -488,7 +488,7 @@
                   <c:v>0.28331679676410071</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6721378395387205</c:v>
+                  <c:v>6.3009201775721602</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.4825105598988066E-2</c:v>
@@ -506,7 +506,7 @@
                   <c:v>8.8497113987194301E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.735867692541735</c:v>
+                  <c:v>10.812610570851437</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2.5065027300464802E-2</c:v>
@@ -5897,7 +5897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EEADE2-A9B3-674B-BA9B-72229A521D77}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -6338,8 +6338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B33892-A41E-4347-B28F-231E96C4EE45}">
   <dimension ref="A2:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6392,7 +6392,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -6442,7 +6442,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -6490,7 +6490,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -6540,7 +6540,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>340699</v>
       </c>
       <c r="H6">
-        <v>658443</v>
+        <v>661062</v>
       </c>
       <c r="I6">
         <v>1672590</v>
@@ -6578,7 +6578,7 @@
         <v>4941547</v>
       </c>
       <c r="N6">
-        <v>10256858</v>
+        <v>10986512</v>
       </c>
       <c r="O6">
         <v>26444568</v>
@@ -6588,7 +6588,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -6638,7 +6638,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -6686,182 +6686,179 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <f t="shared" ref="C9:P9" si="0">100*((C4-C6)/C4)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <f t="shared" si="0"/>
         <v>0.28331679676410071</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <f t="shared" si="0"/>
-        <v>6.6721378395387205</v>
-      </c>
-      <c r="I9" s="15">
+        <v>6.3009201775721602</v>
+      </c>
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
         <v>1.4825105598988066E-2</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="14">
         <f t="shared" si="0"/>
         <v>0.21084435931048381</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="14">
         <f t="shared" si="0"/>
         <v>0.12111948505301814</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="14">
         <f t="shared" si="0"/>
         <v>4.0020902606961082</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <f t="shared" si="0"/>
         <v>8.8497113987194301E-2</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="14">
         <f t="shared" si="0"/>
-        <v>16.735867692541735</v>
-      </c>
-      <c r="O9" s="15">
+        <v>10.812610570851437</v>
+      </c>
+      <c r="O9" s="14">
         <f t="shared" si="0"/>
         <v>2.5065027300464802E-2</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="14">
         <f t="shared" si="0"/>
         <v>2.4661736476073174E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <f t="shared" ref="C11:P11" si="1">100*((C4-C8)/C4)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <f t="shared" si="1"/>
         <v>1.0851631997006446</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="14">
         <f t="shared" si="1"/>
         <v>2.3672346037093849E-2</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="14">
         <f t="shared" si="1"/>
         <v>2.3495459874602515E-2</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="14">
         <f t="shared" si="1"/>
         <v>4.1650458033726358E-3</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="14">
         <f t="shared" si="1"/>
         <v>7.0374062210216401E-2</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="14">
         <f t="shared" si="1"/>
         <v>1.1870917907007463E-3</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="14">
         <f t="shared" si="1"/>
         <v>1.0179336691022478E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
@@ -6878,14 +6875,17 @@
     <mergeCell ref="P11:P12"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="N11:N12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6901,7 +6901,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A4"/>
+      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6912,50 +6912,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20" t="s">
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20" t="s">
+      <c r="T1" s="18"/>
+      <c r="U1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20" t="s">
+      <c r="V1" s="18"/>
+      <c r="W1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="20"/>
+      <c r="X1" s="18"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C2" s="10" t="s">
@@ -7026,7 +7026,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -7100,7 +7100,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -7172,7 +7172,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -7246,7 +7246,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -7318,7 +7318,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -7392,7 +7392,7 @@
       </c>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -7464,935 +7464,960 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="17">
         <f>100*(C4-C6)/C4</f>
         <v>0</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="17">
         <f t="shared" ref="D9:X9" si="0">100*(D4-D6)/D4</f>
         <v>0</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="17">
         <f t="shared" si="0"/>
         <v>0.28527957398250287</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="17">
         <f t="shared" si="0"/>
         <v>0.28527957398250287</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="17">
         <f t="shared" si="0"/>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="17">
         <f t="shared" si="0"/>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="17">
         <f t="shared" si="0"/>
         <v>6.0101272646758694</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="17">
         <f t="shared" si="0"/>
         <v>6.0101272646758694</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="17">
         <f t="shared" si="0"/>
         <v>0.37049121158992121</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="17">
         <f t="shared" si="0"/>
         <v>0.37049121158992121</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q9" s="17">
         <f t="shared" si="0"/>
         <v>0.32912008246667857</v>
       </c>
-      <c r="R9" s="19">
+      <c r="R9" s="17">
         <f t="shared" si="0"/>
         <v>0.32767972407946205</v>
       </c>
-      <c r="S9" s="19">
+      <c r="S9" s="17">
         <f t="shared" si="0"/>
         <v>1.020697822329222</v>
       </c>
-      <c r="T9" s="19">
+      <c r="T9" s="17">
         <f t="shared" si="0"/>
         <v>1.020697822329222</v>
       </c>
-      <c r="U9" s="19">
+      <c r="U9" s="17">
         <f t="shared" si="0"/>
         <v>0.42842809710485213</v>
       </c>
-      <c r="V9" s="19">
+      <c r="V9" s="17">
         <f t="shared" si="0"/>
         <v>0.42935501588230851</v>
       </c>
-      <c r="W9" s="19">
+      <c r="W9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X9" s="19">
+      <c r="X9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="16">
         <f>100*(C4-C8)/C4</f>
         <v>0</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <f t="shared" ref="D11:X11" si="1">100*(D4-D8)/D4</f>
         <v>0</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="16">
         <f t="shared" si="1"/>
         <v>0.27955871310575869</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="16">
         <f t="shared" si="1"/>
         <v>0.28803018926047863</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="Q11" s="16">
         <f t="shared" si="1"/>
         <v>2.1435556047957841E-2</v>
       </c>
-      <c r="R11" s="18">
+      <c r="R11" s="16">
         <f t="shared" si="1"/>
         <v>3.3177421530279964E-2</v>
       </c>
-      <c r="S11" s="18">
+      <c r="S11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T11" s="18">
+      <c r="T11" s="16">
         <f t="shared" si="1"/>
         <v>1.6827101290370412E-2</v>
       </c>
-      <c r="U11" s="18">
+      <c r="U11" s="16">
         <f t="shared" si="1"/>
         <v>-9.3091571075414514E-4</v>
       </c>
-      <c r="V11" s="18">
+      <c r="V11" s="16">
         <f t="shared" si="1"/>
         <v>8.688465751412652E-3</v>
       </c>
-      <c r="W11" s="18">
+      <c r="W11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X11" s="18">
+      <c r="X11" s="16">
         <f t="shared" si="1"/>
         <v>5.6246789245780558E-3</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="19">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19">
         <f>E9</f>
         <v>0</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19">
         <f>G9</f>
         <v>0.28527957398250287</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16">
+      <c r="H14" s="19"/>
+      <c r="I14" s="19">
         <f>I9</f>
         <v>0</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16">
+      <c r="J14" s="19"/>
+      <c r="K14" s="19">
         <f>K9</f>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16">
+      <c r="L14" s="19"/>
+      <c r="M14" s="19">
         <f>M9</f>
         <v>6.0101272646758694</v>
       </c>
-      <c r="N14" s="17"/>
-      <c r="O14" s="16">
+      <c r="N14" s="20"/>
+      <c r="O14" s="19">
         <f>O9</f>
         <v>0.37049121158992121</v>
       </c>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="16">
+      <c r="P14" s="20"/>
+      <c r="Q14" s="19">
         <f>Q9</f>
         <v>0.32912008246667857</v>
       </c>
-      <c r="R14" s="17"/>
-      <c r="S14" s="16">
+      <c r="R14" s="20"/>
+      <c r="S14" s="19">
         <f>S9</f>
         <v>1.020697822329222</v>
       </c>
-      <c r="T14" s="17"/>
-      <c r="U14" s="16">
+      <c r="T14" s="20"/>
+      <c r="U14" s="19">
         <f>U9</f>
         <v>0.42842809710485213</v>
       </c>
-      <c r="V14" s="17"/>
-      <c r="W14" s="16">
+      <c r="V14" s="20"/>
+      <c r="W14" s="19">
         <f>W9</f>
         <v>0</v>
       </c>
-      <c r="X14" s="17"/>
+      <c r="X14" s="20"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="19">
         <f>D9</f>
         <v>0</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16">
+      <c r="D15" s="19"/>
+      <c r="E15" s="19">
         <f>F9</f>
         <v>0</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19">
         <f>H9</f>
         <v>0.28527957398250287</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16">
+      <c r="H15" s="19"/>
+      <c r="I15" s="19">
         <f>J9</f>
         <v>0</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16">
+      <c r="J15" s="19"/>
+      <c r="K15" s="19">
         <f>L9</f>
         <v>3.6421027072963456E-3</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16">
+      <c r="L15" s="19"/>
+      <c r="M15" s="19">
         <f>N9</f>
         <v>6.0101272646758694</v>
       </c>
-      <c r="N15" s="17"/>
-      <c r="O15" s="16">
+      <c r="N15" s="20"/>
+      <c r="O15" s="19">
         <f>P9</f>
         <v>0.37049121158992121</v>
       </c>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="16">
+      <c r="P15" s="20"/>
+      <c r="Q15" s="19">
         <f>R9</f>
         <v>0.32767972407946205</v>
       </c>
-      <c r="R15" s="17"/>
-      <c r="S15" s="16">
+      <c r="R15" s="20"/>
+      <c r="S15" s="19">
         <f>T9</f>
         <v>1.020697822329222</v>
       </c>
-      <c r="T15" s="17"/>
-      <c r="U15" s="16">
+      <c r="T15" s="20"/>
+      <c r="U15" s="19">
         <f>V9</f>
         <v>0.42935501588230851</v>
       </c>
-      <c r="V15" s="17"/>
-      <c r="W15" s="16">
+      <c r="V15" s="20"/>
+      <c r="W15" s="19">
         <f>X9</f>
         <v>0</v>
       </c>
-      <c r="X15" s="17"/>
+      <c r="X15" s="20"/>
     </row>
     <row r="17" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="19">
         <f>C11</f>
         <v>0</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19">
         <f>E11</f>
         <v>0</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16">
+      <c r="F17" s="19"/>
+      <c r="G17" s="19">
         <f>G11</f>
         <v>0</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16">
+      <c r="H17" s="19"/>
+      <c r="I17" s="19">
         <f>I11</f>
         <v>0</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16">
+      <c r="J17" s="19"/>
+      <c r="K17" s="19">
         <f>K11</f>
         <v>0</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16">
+      <c r="L17" s="19"/>
+      <c r="M17" s="19">
         <f>M11</f>
         <v>0.27955871310575869</v>
       </c>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16">
+      <c r="N17" s="19"/>
+      <c r="O17" s="19">
         <f>O11</f>
         <v>0</v>
       </c>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16">
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19">
         <f>Q11</f>
         <v>2.1435556047957841E-2</v>
       </c>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16">
+      <c r="R17" s="19"/>
+      <c r="S17" s="19">
         <f>S11</f>
         <v>0</v>
       </c>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16">
+      <c r="T17" s="19"/>
+      <c r="U17" s="19">
         <f>U11</f>
         <v>-9.3091571075414514E-4</v>
       </c>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16">
+      <c r="V17" s="19"/>
+      <c r="W17" s="19">
         <f>W11</f>
         <v>0</v>
       </c>
-      <c r="X17" s="16"/>
+      <c r="X17" s="19"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="19">
         <f>D12</f>
         <v>0</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16">
+      <c r="D18" s="19"/>
+      <c r="E18" s="19">
         <f>F12</f>
         <v>0</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16">
+      <c r="F18" s="19"/>
+      <c r="G18" s="19">
         <f>H11</f>
         <v>0</v>
       </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16">
+      <c r="H18" s="19"/>
+      <c r="I18" s="19">
         <f>J11</f>
         <v>0</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16">
+      <c r="J18" s="19"/>
+      <c r="K18" s="19">
         <f>L11</f>
         <v>0</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16">
+      <c r="L18" s="19"/>
+      <c r="M18" s="19">
         <f>N11</f>
         <v>0.28803018926047863</v>
       </c>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16">
+      <c r="N18" s="19"/>
+      <c r="O18" s="19">
         <f>P11</f>
         <v>0</v>
       </c>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16">
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19">
         <f>R11</f>
         <v>3.3177421530279964E-2</v>
       </c>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16">
+      <c r="R18" s="19"/>
+      <c r="S18" s="19">
         <f>T11</f>
         <v>1.6827101290370412E-2</v>
       </c>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16">
+      <c r="T18" s="19"/>
+      <c r="U18" s="19">
         <f>V11</f>
         <v>8.688465751412652E-3</v>
       </c>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16">
+      <c r="V18" s="19"/>
+      <c r="W18" s="19">
         <f>X11</f>
         <v>5.6246789245780558E-3</v>
       </c>
-      <c r="X18" s="16"/>
+      <c r="X18" s="19"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="19">
         <f>C5</f>
         <v>0.67100000000000004</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19">
         <f>E5</f>
         <v>1.6584000000000001</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19">
         <f>G5</f>
         <v>2.7709999999999999</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16">
+      <c r="H20" s="19"/>
+      <c r="I20" s="19">
         <f>I5</f>
         <v>15.633800000000001</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16">
+      <c r="J20" s="19"/>
+      <c r="K20" s="19">
         <f>K5</f>
         <v>32.877600000000001</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16">
+      <c r="L20" s="19"/>
+      <c r="M20" s="19">
         <f>M5</f>
         <v>64.142099999999999</v>
       </c>
-      <c r="N20" s="17"/>
-      <c r="O20" s="16">
+      <c r="N20" s="20"/>
+      <c r="O20" s="19">
         <f>O5</f>
         <v>70.239199999999997</v>
       </c>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="16">
+      <c r="P20" s="20"/>
+      <c r="Q20" s="19">
         <f>Q5</f>
         <v>128.3947</v>
       </c>
-      <c r="R20" s="17"/>
-      <c r="S20" s="16">
+      <c r="R20" s="20"/>
+      <c r="S20" s="19">
         <f>S5</f>
         <v>142.79310000000001</v>
       </c>
-      <c r="T20" s="17"/>
-      <c r="U20" s="16">
+      <c r="T20" s="20"/>
+      <c r="U20" s="19">
         <f>U5</f>
         <v>903.16920000000005</v>
       </c>
-      <c r="V20" s="17"/>
-      <c r="W20" s="16">
+      <c r="V20" s="20"/>
+      <c r="W20" s="19">
         <f>W5</f>
         <v>2534.8456999999999</v>
       </c>
-      <c r="X20" s="17"/>
+      <c r="X20" s="20"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="19">
         <f>D5</f>
         <v>0.39979999999999999</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16">
+      <c r="D21" s="19"/>
+      <c r="E21" s="19">
         <f>F5</f>
         <v>1.1163000000000001</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19">
         <f>H5</f>
         <v>1.3845000000000001</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16">
+      <c r="H21" s="19"/>
+      <c r="I21" s="19">
         <f>J5</f>
         <v>8.7070000000000007</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16">
+      <c r="J21" s="19"/>
+      <c r="K21" s="19">
         <f>L5</f>
         <v>14.837</v>
       </c>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16">
+      <c r="L21" s="19"/>
+      <c r="M21" s="19">
         <f>N5</f>
         <v>35.283999999999999</v>
       </c>
-      <c r="N21" s="17"/>
-      <c r="O21" s="16">
+      <c r="N21" s="20"/>
+      <c r="O21" s="19">
         <f>P5</f>
         <v>33.219700000000003</v>
       </c>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="16">
+      <c r="P21" s="20"/>
+      <c r="Q21" s="19">
         <f>R5</f>
         <v>63.618000000000002</v>
       </c>
-      <c r="R21" s="17"/>
-      <c r="S21" s="16">
+      <c r="R21" s="20"/>
+      <c r="S21" s="19">
         <f>T5</f>
         <v>61.295900000000003</v>
       </c>
-      <c r="T21" s="17"/>
-      <c r="U21" s="16">
+      <c r="T21" s="20"/>
+      <c r="U21" s="19">
         <f>V5</f>
         <v>448.58699999999999</v>
       </c>
-      <c r="V21" s="17"/>
-      <c r="W21" s="16">
+      <c r="V21" s="20"/>
+      <c r="W21" s="19">
         <f>X5</f>
         <v>1474.5264</v>
       </c>
-      <c r="X21" s="17"/>
+      <c r="X21" s="20"/>
     </row>
     <row r="23" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="19">
         <f>C7</f>
         <v>1.625</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16">
+      <c r="D23" s="19"/>
+      <c r="E23" s="19">
         <f>E7</f>
         <v>3.5937999999999999</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19">
         <f>G7</f>
         <v>5.7656000000000001</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16">
+      <c r="H23" s="19"/>
+      <c r="I23" s="19">
         <f>I7</f>
         <v>35.382899999999999</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16">
+      <c r="J23" s="19"/>
+      <c r="K23" s="19">
         <f>K7</f>
         <v>64.046899999999994</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16">
+      <c r="L23" s="19"/>
+      <c r="M23" s="19">
         <f>M7</f>
         <v>188.39060000000001</v>
       </c>
-      <c r="N23" s="17"/>
-      <c r="O23" s="16">
+      <c r="N23" s="20"/>
+      <c r="O23" s="19">
         <f>O7</f>
         <v>216.10939999999999</v>
       </c>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="16">
+      <c r="P23" s="20"/>
+      <c r="Q23" s="19">
         <f>Q7</f>
         <v>311.26560000000001</v>
       </c>
-      <c r="R23" s="17"/>
-      <c r="S23" s="16">
+      <c r="R23" s="20"/>
+      <c r="S23" s="19">
         <f>S7</f>
         <v>365.04689999999999</v>
       </c>
-      <c r="T23" s="17"/>
-      <c r="U23" s="16">
+      <c r="T23" s="20"/>
+      <c r="U23" s="19">
         <f>U7</f>
         <v>1575.6561999999999</v>
       </c>
-      <c r="V23" s="17"/>
-      <c r="W23" s="16">
+      <c r="V23" s="20"/>
+      <c r="W23" s="19">
         <f>W7</f>
         <v>2794.1891000000001</v>
       </c>
-      <c r="X23" s="17"/>
+      <c r="X23" s="20"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="19">
         <f>D7</f>
         <v>1.875</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16">
+      <c r="D24" s="19"/>
+      <c r="E24" s="19">
         <f>F7</f>
         <v>4.4062000000000001</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16">
+      <c r="F24" s="19"/>
+      <c r="G24" s="19">
         <f>H7</f>
         <v>7.5156000000000001</v>
       </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16">
+      <c r="H24" s="19"/>
+      <c r="I24" s="19">
         <f>J7</f>
         <v>44.488599999999998</v>
       </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16">
+      <c r="J24" s="19"/>
+      <c r="K24" s="19">
         <f>L7</f>
         <v>80.75</v>
       </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16">
+      <c r="L24" s="19"/>
+      <c r="M24" s="19">
         <f>N7</f>
         <v>224.54689999999999</v>
       </c>
-      <c r="N24" s="17"/>
-      <c r="O24" s="16">
+      <c r="N24" s="20"/>
+      <c r="O24" s="19">
         <f>P7</f>
         <v>271.32810000000001</v>
       </c>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="16">
+      <c r="P24" s="20"/>
+      <c r="Q24" s="19">
         <f>R7</f>
         <v>387.5</v>
       </c>
-      <c r="R24" s="17"/>
-      <c r="S24" s="16">
+      <c r="R24" s="20"/>
+      <c r="S24" s="19">
         <f>T7</f>
         <v>440.04689999999999</v>
       </c>
-      <c r="T24" s="17"/>
-      <c r="U24" s="16">
+      <c r="T24" s="20"/>
+      <c r="U24" s="19">
         <f>V7</f>
         <v>2883.3281000000002</v>
       </c>
-      <c r="V24" s="17"/>
-      <c r="W24" s="16">
+      <c r="V24" s="20"/>
+      <c r="W24" s="19">
         <f>X7</f>
         <v>3410.9778999999999</v>
       </c>
-      <c r="X24" s="17"/>
+      <c r="X24" s="20"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="19">
         <f>C3</f>
         <v>1.5461</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="16">
+      <c r="D26" s="20"/>
+      <c r="E26" s="19">
         <f>E3</f>
         <v>3.9401000000000002</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="16">
+      <c r="F26" s="20"/>
+      <c r="G26" s="19">
         <f>G3</f>
         <v>6.3446999999999996</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="16">
+      <c r="H26" s="20"/>
+      <c r="I26" s="19">
         <f>I3</f>
         <v>38.189</v>
       </c>
-      <c r="J26" s="17"/>
-      <c r="K26" s="16">
+      <c r="J26" s="20"/>
+      <c r="K26" s="19">
         <f>K3</f>
         <v>72.674499999999995</v>
       </c>
-      <c r="L26" s="17"/>
-      <c r="M26" s="16">
+      <c r="L26" s="20"/>
+      <c r="M26" s="19">
         <f>M3</f>
         <v>161.48249999999999</v>
       </c>
-      <c r="N26" s="17"/>
-      <c r="O26" s="16">
+      <c r="N26" s="20"/>
+      <c r="O26" s="19">
         <f>O3</f>
         <v>223.24950000000001</v>
       </c>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="16">
+      <c r="P26" s="20"/>
+      <c r="Q26" s="19">
         <f>Q3</f>
         <v>324.71039999999999</v>
       </c>
-      <c r="R26" s="17"/>
-      <c r="S26" s="16">
+      <c r="R26" s="20"/>
+      <c r="S26" s="19">
         <f>S3</f>
         <v>464.81439999999998</v>
       </c>
-      <c r="T26" s="17"/>
-      <c r="U26" s="16">
+      <c r="T26" s="20"/>
+      <c r="U26" s="19">
         <f>U3</f>
         <v>1655.0168000000001</v>
       </c>
-      <c r="V26" s="17"/>
-      <c r="W26" s="16">
+      <c r="V26" s="20"/>
+      <c r="W26" s="19">
         <f>W3</f>
         <v>3689.8222000000001</v>
       </c>
-      <c r="X26" s="17"/>
+      <c r="X26" s="20"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="15"/>
       <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="19">
         <f>D3</f>
         <v>1.9312</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="16">
+      <c r="D27" s="20"/>
+      <c r="E27" s="19">
         <f>F3</f>
         <v>5.1288999999999998</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="16">
+      <c r="F27" s="20"/>
+      <c r="G27" s="19">
         <f>H3</f>
         <v>8.5748999999999995</v>
       </c>
-      <c r="H27" s="17"/>
-      <c r="I27" s="16">
+      <c r="H27" s="20"/>
+      <c r="I27" s="19">
         <f>J3</f>
         <v>48.531300000000002</v>
       </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="16">
+      <c r="J27" s="20"/>
+      <c r="K27" s="19">
         <f>L3</f>
         <v>93.75</v>
       </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="16">
+      <c r="L27" s="20"/>
+      <c r="M27" s="19">
         <f>N3</f>
         <v>225.67140000000001</v>
       </c>
-      <c r="N27" s="17"/>
-      <c r="O27" s="16">
+      <c r="N27" s="20"/>
+      <c r="O27" s="19">
         <f>P3</f>
         <v>301.35610000000003</v>
       </c>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="16">
+      <c r="P27" s="20"/>
+      <c r="Q27" s="19">
         <f>R3</f>
         <v>478.46609999999998</v>
       </c>
-      <c r="R27" s="17"/>
-      <c r="S27" s="16">
+      <c r="R27" s="20"/>
+      <c r="S27" s="19">
         <f>T3</f>
         <v>580.44349999999997</v>
       </c>
-      <c r="T27" s="17"/>
-      <c r="U27" s="16">
+      <c r="T27" s="20"/>
+      <c r="U27" s="19">
         <f>V3</f>
         <v>2248.9456</v>
       </c>
-      <c r="V27" s="17"/>
-      <c r="W27" s="16">
+      <c r="V27" s="20"/>
+      <c r="W27" s="19">
         <f>X3</f>
         <v>5671.4978000000001</v>
       </c>
-      <c r="X27" s="17"/>
+      <c r="X27" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="177">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="M18:N18"/>
@@ -8417,95 +8442,70 @@
     <mergeCell ref="W14:X14"/>
     <mergeCell ref="U14:V14"/>
     <mergeCell ref="S14:T14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>